<commit_message>
Schema changed. Updated ExecutionPlaces.xlsx. Implemented statistics by records/assignments
</commit_message>
<xml_diff>
--- a/DatabaseUpdate/ExcelFiles/ExecutionPlaces.xlsx
+++ b/DatabaseUpdate/ExcelFiles/ExecutionPlaces.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <x:si>
     <x:t>Id</x:t>
   </x:si>
@@ -49,36 +49,39 @@
     <x:t>True</x:t>
   </x:si>
   <x:si>
+    <x:t>|DayStationary|</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Амбулаторно</x:t>
+  </x:si>
+  <x:si>
+    <x:t>амбул</x:t>
+  </x:si>
+  <x:si>
+    <x:t>амбулаторно</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|Polyclinic|</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Скорая неотложная помощь</x:t>
+  </x:si>
+  <x:si>
+    <x:t>бриг СМП</x:t>
+  </x:si>
+  <x:si>
+    <x:t>в условиях скорой неотложной помощи</x:t>
+  </x:si>
+  <x:si>
     <x:t>NULL</x:t>
   </x:si>
   <x:si>
-    <x:t>3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Амбулаторно</x:t>
-  </x:si>
-  <x:si>
-    <x:t>амбул</x:t>
-  </x:si>
-  <x:si>
-    <x:t>амбулаторно</x:t>
-  </x:si>
-  <x:si>
-    <x:t>|Polyclinic|</x:t>
-  </x:si>
-  <x:si>
-    <x:t>4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Скорая неотложная помощь</x:t>
-  </x:si>
-  <x:si>
-    <x:t>бриг СМП</x:t>
-  </x:si>
-  <x:si>
-    <x:t>в условиях скорой неотложной помощи</x:t>
-  </x:si>
-  <x:si>
     <x:t>6</x:t>
   </x:si>
   <x:si>
@@ -89,6 +92,9 @@
   </x:si>
   <x:si>
     <x:t>в условиях стационара</x:t>
+  </x:si>
+  <x:si>
+    <x:t>|Stationary|</x:t>
   </x:si>
   <x:si>
     <x:t>8</x:t>
@@ -534,47 +540,47 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="F4" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:6">
       <x:c r="A5" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="C5" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="D5" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="E5" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
       <x:c r="F5" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>26</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:6">
       <x:c r="A6" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="C6" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="E6" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
       <x:c r="F6" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>